<commit_message>
chosses pour le rapport
</commit_message>
<xml_diff>
--- a/results/Results_2.xlsx
+++ b/results/Results_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flash\Documents\CODE\blobwar\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{976A7A0B-5648-4F34-BD7A-71CE3A17A7ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E687359D-70E8-4C6F-9948-C91EC6A414B5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{0EDCD334-53E2-4E89-91CE-387F55CEFB2B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{0EDCD334-53E2-4E89-91CE-387F55CEFB2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Temps du Jeu" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -177,17 +184,409 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -318,7 +717,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Temps du Jeu'!$A$3:$A$22</c:f>
+              <c:f>'Temps du Jeu'!$B$4:$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
@@ -386,10 +785,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Temps du Jeu'!$F$3:$F$22</c:f>
+              <c:f>'Temps du Jeu'!$G$4:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2.3E-3</c:v>
                 </c:pt>
@@ -431,24 +830,6 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1.0048999999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.8248000000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.2972999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>6.3537999999999997</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9.0739999999999998</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>20.432400000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>167.31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -626,6 +1007,367 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Temps</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-AR" baseline="0"/>
+              <a:t> de Jeu</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Temps du Jeu'!$B$17:$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>AlphaBeta4 vs Greedy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MinMax3 vs Greedy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AlphaBeta3 vs MinMax3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MinMax3 vs MinMax2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MinMax3 vs MinMax3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AlphaBeta5 vs Greedy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Temps du Jeu'!$B$17:$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>AlphaBeta4 vs Greedy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MinMax3 vs Greedy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AlphaBeta3 vs MinMax3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MinMax3 vs MinMax2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MinMax3 vs MinMax3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AlphaBeta5 vs Greedy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Temps du Jeu'!$G$17:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0048999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8248000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2972999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.3537999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0739999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.432400000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DAAC-413E-8B21-9687C0D61427}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="362868256"/>
+        <c:axId val="362867272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="362868256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362867272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="362867272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362868256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -1119,6 +1861,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
@@ -1589,6 +2371,475 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700">
+        <a:solidFill>
+          <a:schemeClr val="lt2"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2095,16 +3346,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2124,6 +3375,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{275623EF-E704-441D-B963-A310CF89A095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2470,449 +3759,526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE3CC6B-4316-43AA-A499-CA10F70E9375}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
-        <v>255</v>
-      </c>
-      <c r="C3">
-        <v>212</v>
-      </c>
-      <c r="D3">
+      <c r="C4" s="13">
+        <v>51</v>
+      </c>
+      <c r="D4" s="14">
+        <v>42</v>
+      </c>
+      <c r="E4" s="15">
+        <v>7</v>
+      </c>
+      <c r="F4" s="16">
+        <v>500</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2.3E-3</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18">
+        <v>100</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21">
+        <v>100</v>
+      </c>
+      <c r="G5" s="22">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="18">
+        <v>61</v>
+      </c>
+      <c r="D6" s="19">
         <v>33</v>
       </c>
-      <c r="E3">
+      <c r="E6" s="20">
+        <v>6</v>
+      </c>
+      <c r="F6" s="21">
+        <v>100</v>
+      </c>
+      <c r="G6" s="22">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="18">
+        <v>100</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21">
+        <v>100</v>
+      </c>
+      <c r="G7" s="22">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="18">
+        <v>81</v>
+      </c>
+      <c r="D8" s="19">
+        <v>14</v>
+      </c>
+      <c r="E8" s="20">
+        <v>5</v>
+      </c>
+      <c r="F8" s="21">
         <v>500</v>
       </c>
-      <c r="F3">
-        <v>2.3E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
+      <c r="G8" s="22">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="18">
         <v>100</v>
       </c>
-      <c r="C4">
+      <c r="D9" s="19">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="E9" s="20">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="F9" s="21">
         <v>100</v>
       </c>
-      <c r="F4">
-        <v>2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="G9" s="22">
+        <v>1.61E-2</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>100</v>
+      </c>
+      <c r="D10" s="19">
         <v>0</v>
       </c>
-      <c r="B5">
-        <v>61</v>
-      </c>
-      <c r="C5">
-        <v>33</v>
-      </c>
-      <c r="D5">
+      <c r="E10" s="20">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21">
+        <v>100</v>
+      </c>
+      <c r="G10" s="22">
+        <v>1.8499999999999999E-2</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="18">
+        <v>100</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0</v>
+      </c>
+      <c r="F11" s="21">
+        <v>500</v>
+      </c>
+      <c r="G11" s="22">
+        <v>6.8599999999999994E-2</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="18">
+        <v>100</v>
+      </c>
+      <c r="D12" s="19">
+        <v>0</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0</v>
+      </c>
+      <c r="F12" s="21">
+        <v>100</v>
+      </c>
+      <c r="G12" s="22">
+        <v>0.14660000000000001</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="18">
+        <v>100</v>
+      </c>
+      <c r="D13" s="19">
+        <v>0</v>
+      </c>
+      <c r="E13" s="20">
+        <v>0</v>
+      </c>
+      <c r="F13" s="21">
+        <v>100</v>
+      </c>
+      <c r="G13" s="22">
+        <v>0.16880000000000001</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="C14" s="18">
         <v>100</v>
       </c>
-      <c r="F5">
-        <v>5.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
+      <c r="D14" s="19">
+        <v>0</v>
+      </c>
+      <c r="E14" s="20">
+        <v>0</v>
+      </c>
+      <c r="F14" s="21">
         <v>100</v>
       </c>
-      <c r="C6">
+      <c r="G14" s="22">
+        <v>0.39389999999999997</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="18">
+        <v>100</v>
+      </c>
+      <c r="D15" s="19">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="E15" s="20">
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="F15" s="21">
         <v>100</v>
       </c>
-      <c r="F6">
-        <v>7.7999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>406</v>
-      </c>
-      <c r="C7">
-        <v>73</v>
-      </c>
-      <c r="D7">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>500</v>
-      </c>
-      <c r="F7">
-        <v>8.2000000000000007E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="G15" s="22">
+        <v>0.56640000000000001</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="18">
+        <v>100</v>
+      </c>
+      <c r="D16" s="19">
+        <v>0</v>
+      </c>
+      <c r="E16" s="20">
+        <v>0</v>
+      </c>
+      <c r="F16" s="21">
+        <v>25</v>
+      </c>
+      <c r="G16" s="22">
+        <v>0.8286</v>
+      </c>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="18">
+        <v>100</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0</v>
+      </c>
+      <c r="E17" s="20">
+        <v>0</v>
+      </c>
+      <c r="F17" s="21">
+        <v>100</v>
+      </c>
+      <c r="G17" s="22">
+        <v>1.0048999999999999</v>
+      </c>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18">
+        <v>100</v>
+      </c>
+      <c r="D18" s="19">
+        <v>0</v>
+      </c>
+      <c r="E18" s="20">
+        <v>0</v>
+      </c>
+      <c r="F18" s="21">
+        <v>120</v>
+      </c>
+      <c r="G18" s="22">
+        <v>3.8248000000000002</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="18">
+        <v>0</v>
+      </c>
+      <c r="D19" s="19">
+        <v>100</v>
+      </c>
+      <c r="E19" s="20">
+        <v>0</v>
+      </c>
+      <c r="F19" s="21">
+        <v>5</v>
+      </c>
+      <c r="G19" s="22">
+        <v>5.2972999999999999</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="18">
+        <v>100</v>
+      </c>
+      <c r="D20" s="19">
+        <v>0</v>
+      </c>
+      <c r="E20" s="20">
+        <v>0</v>
+      </c>
+      <c r="F20" s="21">
+        <v>50</v>
+      </c>
+      <c r="G20" s="22">
+        <v>6.3537999999999997</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="18">
+        <v>100</v>
+      </c>
+      <c r="D21" s="19">
+        <v>0</v>
+      </c>
+      <c r="E21" s="20">
+        <v>0</v>
+      </c>
+      <c r="F21" s="21">
+        <v>32</v>
+      </c>
+      <c r="G21" s="22">
+        <v>9.0739999999999998</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="18">
+        <v>100</v>
+      </c>
+      <c r="D22" s="19">
+        <v>0</v>
+      </c>
+      <c r="E22" s="20">
+        <v>0</v>
+      </c>
+      <c r="F22" s="21">
+        <v>10</v>
+      </c>
+      <c r="G22" s="22">
+        <v>20.432400000000001</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="23">
+        <v>100</v>
+      </c>
+      <c r="D23" s="24">
+        <v>0</v>
+      </c>
+      <c r="E23" s="25">
+        <v>0</v>
+      </c>
+      <c r="F23" s="26">
         <v>3</v>
       </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-      <c r="F8">
-        <v>1.61E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>100</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-      <c r="F9">
-        <v>1.8499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>500</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>500</v>
-      </c>
-      <c r="F10">
-        <v>6.8599999999999994E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>100</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>100</v>
-      </c>
-      <c r="F11">
-        <v>0.14660000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>100</v>
-      </c>
-      <c r="F12">
-        <v>0.16880000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>100</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>100</v>
-      </c>
-      <c r="F13">
-        <v>0.39389999999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>100</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>100</v>
-      </c>
-      <c r="F14">
-        <v>0.56640000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>25</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>25</v>
-      </c>
-      <c r="F15">
-        <v>0.8286</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16">
-        <v>100</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>100</v>
-      </c>
-      <c r="F16">
-        <v>1.0048999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>120</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>120</v>
-      </c>
-      <c r="F17">
-        <v>3.8248000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>5.2972999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>50</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>50</v>
-      </c>
-      <c r="F19">
-        <v>6.3537999999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>32</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>32</v>
-      </c>
-      <c r="F20">
-        <v>9.0739999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21">
-        <v>100</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>10</v>
-      </c>
-      <c r="F21">
-        <v>20.432400000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22">
+      <c r="G23" s="27">
         <v>167.31</v>
       </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A3:F23">
-    <sortCondition ref="F3"/>
+  <sortState ref="B4:G24">
+    <sortCondition ref="G4"/>
   </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="B1:D1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="H2:H24"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="A2:A24"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2920,7 +4286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6442CA0B-B678-4652-9210-41071C2393A7}">
   <dimension ref="A3:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>

</xml_diff>